<commit_message>
adding mse to the final file
</commit_message>
<xml_diff>
--- a/RMSE for Model.xlsx
+++ b/RMSE for Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crew_\OneDrive\Escritorio\Guille\UTSA Masters\MSDA\DA6813\DA6813\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE82D6A1-6E21-45DF-919B-235ECB3DE72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17FBD39-E75D-4053-96DF-FD7EBBFC3FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="-15870" windowWidth="25440" windowHeight="15270" xr2:uid="{40277F77-485A-46B6-8B03-1D3B5A1BA214}"/>
+    <workbookView xWindow="-27195" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{40277F77-485A-46B6-8B03-1D3B5A1BA214}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -212,15 +212,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -261,7 +252,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -269,7 +262,33 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -283,26 +302,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -310,7 +314,37 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -651,7 +685,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" sqref="A1:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -661,399 +695,462 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="11">
         <v>126671324</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="15">
         <v>126671324</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="7">
+        <v>20.05021</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="12">
         <v>32653797</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="16">
         <v>32653800</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="8">
+        <v>17.755682</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="12">
         <v>22107483</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="16">
         <v>22107487</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="8">
+        <v>9.2336460000000002</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="12">
         <v>637938743</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="16">
         <v>637938739</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="F5" s="11"/>
+      <c r="D5" s="8">
+        <v>11.861848999999999</v>
+      </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="12">
         <v>37163364</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="16">
         <v>37163365</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="8">
+        <v>22.258886</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="12">
         <v>382385019</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="16">
         <v>382385017</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="8">
+        <v>17.437448</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="12">
         <v>36898553</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="16">
         <v>36898556</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="F8" s="11"/>
+      <c r="D8" s="8">
+        <v>12.606989</v>
+      </c>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="12">
         <v>26760786</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="16">
         <v>26760786</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="8">
+        <v>12.095190000000001</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="12">
         <v>46218461</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="16">
         <v>46218460</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="8">
+        <v>15.726054</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="12">
         <v>231874886</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="16">
         <v>231874886</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="8">
+        <v>13.213855000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="12">
         <v>51032386</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="16">
         <v>51032386</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="8">
+        <v>7.480315</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="12">
         <v>102925210</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="16">
         <v>102925207</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="8">
+        <v>19.219626999999999</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="12">
         <v>23676034</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="16">
         <v>23676055</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="8">
+        <v>4.8369559999999998</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="12">
         <v>330452414</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="16">
         <v>330452413</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="8">
+        <v>17.140916000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="12">
         <v>58363850</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="16">
         <v>58363852</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="8">
+        <v>8.6910139999999991</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="12">
         <v>146424585</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="16">
         <v>146424583</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="8">
+        <v>9.1362299999999994</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="12">
         <v>35913555</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="16">
         <v>35913557</v>
       </c>
-      <c r="D18" s="4"/>
+      <c r="D18" s="8">
+        <v>3.1621220000000001</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="12">
         <v>45366153</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="16">
         <v>45366156</v>
       </c>
-      <c r="D19" s="4"/>
+      <c r="D19" s="8">
+        <v>7.1216160000000004</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="12">
         <v>24965634</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="16">
         <v>24965638</v>
       </c>
-      <c r="D20" s="4"/>
+      <c r="D20" s="8">
+        <v>6.8786230000000002</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="12">
         <v>15020575</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="16">
         <v>15020577</v>
       </c>
-      <c r="D21" s="4"/>
+      <c r="D21" s="8">
+        <v>8.1892469999999999</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="12">
         <v>65631688</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="16">
         <v>65631691</v>
       </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="8">
+        <v>9.1766400000000008</v>
+      </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="12">
         <v>306000553</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="16">
         <v>306000552</v>
       </c>
-      <c r="D23" s="4"/>
+      <c r="D23" s="8">
+        <v>10.32122</v>
+      </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="12">
         <v>207245099</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="16">
         <v>207245100</v>
       </c>
-      <c r="D24" s="4"/>
+      <c r="D24" s="8">
+        <v>8.2251460000000005</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="12">
         <v>46194506</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="16">
         <v>46194511</v>
       </c>
-      <c r="D25" s="4"/>
+      <c r="D25" s="8">
+        <v>5.7260390000000001</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="12">
         <v>149761089</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="16">
         <v>149761092</v>
       </c>
-      <c r="D26" s="4"/>
+      <c r="D26" s="8">
+        <v>3.8187440000000001</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="12">
         <v>15458994</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="16">
         <v>15458999</v>
       </c>
-      <c r="D27" s="4"/>
+      <c r="D27" s="8">
+        <v>3.5969799999999998</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="12">
         <v>18958828</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="16">
         <v>18958836</v>
       </c>
-      <c r="D28" s="4"/>
+      <c r="D28" s="8">
+        <v>11.641442</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="12">
         <v>65737755</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="16">
         <v>65737756</v>
       </c>
-      <c r="D29" s="4"/>
+      <c r="D29" s="8">
+        <v>5.2101040000000003</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="12">
         <v>51055448</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="16">
         <v>51055449</v>
       </c>
-      <c r="D30" s="4"/>
+      <c r="D30" s="8">
+        <v>3.560991</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="12">
         <v>88060818</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="16">
         <v>88060821</v>
       </c>
-      <c r="D31" s="4"/>
+      <c r="D31" s="8">
+        <v>12.730046</v>
+      </c>
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="13">
         <f>AVERAGE(B2:B31)</f>
         <v>114297253</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="17">
         <f>AVERAGE(C2:C31)</f>
         <v>114297255.03333333</v>
       </c>
-      <c r="D32" s="6" t="e">
+      <c r="D32" s="9">
         <f>AVERAGE(D2:D30)</f>
-        <v>#DIV/0!</v>
+        <v>10.530130379310343</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D32" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>